<commit_message>
defined data from outlier
</commit_message>
<xml_diff>
--- a/analysis_ST/plotsTFE_inotec_P4_depth_plot.pdf.xlsx
+++ b/analysis_ST/plotsTFE_inotec_P4_depth_plot.pdf.xlsx
@@ -592,7 +592,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>10.802132</v>
+        <v>1.428914</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -612,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>15.16492983</v>
+        <v>2.092668</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1071,12 +1071,12 @@
         <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8542755</v>
+        <v>1.428914</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1088,46 +1088,46 @@
         <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>1.0455661</v>
+        <v>2.092668</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5293127</v>
+        <v>0.8542755</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4071637</v>
+        <v>1.0455661</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -1139,29 +1139,29 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7989626</v>
+        <v>0.5293127</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
-        <v>1.9536179</v>
+        <v>0.4071637</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1170,18 +1170,18 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E12" t="n">
-        <v>0.579248</v>
+        <v>0.7989626</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1190,12 +1190,12 @@
         <v>25</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5277763</v>
+        <v>1.9536179</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -1207,46 +1207,46 @@
         <v>25</v>
       </c>
       <c r="E14" t="n">
-        <v>1.3006195</v>
+        <v>0.579248</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
       <c r="E15" t="n">
-        <v>1.856821</v>
+        <v>0.5277763</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
       <c r="E16" t="n">
-        <v>1.6532389</v>
+        <v>1.3006195</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -1258,15 +1258,15 @@
         <v>25</v>
       </c>
       <c r="E17" t="n">
-        <v>1.5095789</v>
+        <v>1.856821</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1275,15 +1275,15 @@
         <v>25</v>
       </c>
       <c r="E18" t="n">
-        <v>1.8045807</v>
+        <v>1.6532389</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -1292,12 +1292,12 @@
         <v>25</v>
       </c>
       <c r="E19" t="n">
-        <v>1.6040717</v>
+        <v>1.5095789</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1309,40 +1309,74 @@
         <v>25</v>
       </c>
       <c r="E20" t="n">
-        <v>3.0191582</v>
+        <v>1.8045807</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
       <c r="E21" t="n">
-        <v>0.581553</v>
+        <v>1.6040717</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0191582</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.581553</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" t="n">
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.6606808</v>
       </c>
     </row>

</xml_diff>